<commit_message>
clear data table, filtered, sorted data table done success
</commit_message>
<xml_diff>
--- a/FindRowsCount_ColCount_ColNames_with_WorkbookActivities1/Data/Sample2_Large_data.xlsx
+++ b/FindRowsCount_ColCount_ColNames_with_WorkbookActivities1/Data/Sample2_Large_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPATH_PRACTICES\UIPATH_8AM_BATCH\WorkBookActivities1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPATH_PRACTICES\UIPATH_8AM_BATCH\FindRowsCount_ColCount_ColNames_with_WorkbookActivities1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F2F31D-1EAC-4BC9-A70D-FF42CDBAD021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D24472F-58D6-4751-9B46-0624CD9D6A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -667,7 +667,7 @@
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>110</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>170</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>